<commit_message>
CardBoard V2 new implementation
Alpha level to 32 bit
</commit_message>
<xml_diff>
--- a/Heures.xlsx
+++ b/Heures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8655" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tâches</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Programmation C++</t>
+  </si>
+  <si>
+    <t>Création nouvelle carte</t>
+  </si>
+  <si>
+    <t>Programmation test carte</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -133,6 +139,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O16"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,51 +472,54 @@
     <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.375" customWidth="1"/>
     <col min="4" max="8" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="3.75" customWidth="1"/>
-    <col min="12" max="12" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.75" customWidth="1"/>
-    <col min="14" max="15" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="3.75" customWidth="1"/>
+    <col min="13" max="13" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.75" customWidth="1"/>
+    <col min="15" max="16" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="4"/>
       <c r="J1" s="5"/>
       <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
-        <f>SUM(D6:V27)</f>
-        <v>30</v>
+        <f>SUM(D6:W28)</f>
+        <v>39.5</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,19 +548,22 @@
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>42604</v>
       </c>
@@ -553,7 +571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>42605</v>
       </c>
@@ -561,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>42606</v>
       </c>
@@ -572,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>42616</v>
       </c>
@@ -580,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>42624</v>
       </c>
@@ -588,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>42641</v>
       </c>
@@ -599,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>42642</v>
       </c>
@@ -613,50 +631,93 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>42642</v>
       </c>
-      <c r="L13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>42643</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>42644</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
         <v>42645</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-      <c r="M16">
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>42653</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>42656</v>
+      </c>
+      <c r="F19">
+        <v>2.5</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.5</v>
+      </c>
+      <c r="L19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>42657</v>
+      </c>
+      <c r="J20">
+        <v>0.5</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:H2"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new Fonction RainbowVertical & On Axis
</commit_message>
<xml_diff>
--- a/Heures.xlsx
+++ b/Heures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tâches</t>
   </si>
@@ -67,13 +67,19 @@
   </si>
   <si>
     <t>Programmation C++</t>
+  </si>
+  <si>
+    <t>Création nouvelle carte</t>
+  </si>
+  <si>
+    <t>Programmation test carte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +98,13 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -134,6 +147,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,62 +471,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O16"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" customWidth="1"/>
-    <col min="4" max="8" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="3.75" customWidth="1"/>
-    <col min="12" max="12" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.75" customWidth="1"/>
-    <col min="14" max="15" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="8" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="3.77734375" customWidth="1"/>
+    <col min="13" max="13" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.77734375" customWidth="1"/>
+    <col min="15" max="16" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="4"/>
       <c r="J1" s="5"/>
       <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
-        <f>SUM(D6:V27)</f>
-        <v>30</v>
+        <f>SUM(D6:W28)</f>
+        <v>39.5</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="156" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,38 +539,41 @@
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>42604</v>
       </c>
@@ -553,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>42605</v>
       </c>
@@ -561,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>42606</v>
       </c>
@@ -572,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>42616</v>
       </c>
@@ -580,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>42624</v>
       </c>
@@ -588,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>42641</v>
       </c>
@@ -599,7 +627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>42642</v>
       </c>
@@ -613,50 +641,93 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>42642</v>
       </c>
-      <c r="L13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>42643</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>42644</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>42645</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-      <c r="M16">
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>42653</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>42656</v>
+      </c>
+      <c r="F19">
+        <v>2.5</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.5</v>
+      </c>
+      <c r="L19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>42657</v>
+      </c>
+      <c r="J20">
+        <v>0.5</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:H2"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>